<commit_message>
correct date from table && changed default focus
</commit_message>
<xml_diff>
--- a/Летальность.xlsx
+++ b/Летальность.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
   <si>
     <t xml:space="preserve">№п\п</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t xml:space="preserve">ХО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01.01.2222</t>
   </si>
   <si>
     <t xml:space="preserve">4-7с</t>
@@ -242,11 +239,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
     <numFmt numFmtId="166" formatCode="[$-409]M/D/YYYY"/>
     <numFmt numFmtId="167" formatCode="[$-409]H:MM"/>
+    <numFmt numFmtId="168" formatCode="D&quot;. &quot;MMM&quot;. &quot;YYYY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -367,7 +365,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -392,6 +390,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -405,6 +407,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -431,10 +437,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF6"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -549,7 +555,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
@@ -571,11 +577,11 @@
       <c r="G2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="H2" s="6" t="n">
         <v>44644</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>37</v>
+      <c r="I2" s="7" t="n">
+        <v>117610</v>
       </c>
       <c r="J2" s="5" t="n">
         <v>1</v>
@@ -584,49 +590,49 @@
         <v>5</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="5"/>
+      <c r="N2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="7" t="n">
+        <v>43467</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="6" t="n">
-        <v>43467</v>
-      </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="W2" s="5"/>
       <c r="X2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y2" s="5"/>
       <c r="Z2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA2" s="5"/>
-      <c r="AB2" s="6" t="n">
+      <c r="AB2" s="7" t="n">
         <v>43467</v>
       </c>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AE2" s="5"/>
       <c r="AF2" s="5" t="n">
@@ -638,16 +644,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>37</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>35</v>
@@ -658,7 +664,7 @@
       <c r="H3" s="5" t="n">
         <v>12486</v>
       </c>
-      <c r="I3" s="6" t="n">
+      <c r="I3" s="7" t="n">
         <v>43466</v>
       </c>
       <c r="J3" s="5" t="n">
@@ -668,35 +674,35 @@
         <v>5</v>
       </c>
       <c r="L3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="10" t="n">
+        <v>0.190972222222222</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="7" t="n">
+        <v>43467</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="9" t="n">
-        <v>0.190972222222222</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="6" t="n">
-        <v>43467</v>
-      </c>
-      <c r="R3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="U3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="W3" s="5" t="n">
         <v>1</v>
@@ -704,15 +710,15 @@
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
       <c r="Z3" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA3" s="5"/>
-      <c r="AB3" s="6" t="n">
+      <c r="AB3" s="7" t="n">
         <v>43467</v>
       </c>
       <c r="AC3" s="5"/>
       <c r="AD3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AE3" s="5"/>
       <c r="AF3" s="5" t="n">
@@ -724,7 +730,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>33</v>
@@ -733,19 +739,19 @@
         <v>80</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="H4" s="5" t="n">
         <v>24122</v>
       </c>
-      <c r="I4" s="6" t="n">
-        <v>-1</v>
+      <c r="I4" s="7" t="n">
+        <v>36523</v>
       </c>
       <c r="J4" s="5" t="n">
         <v>1</v>
@@ -754,28 +760,28 @@
         <v>5</v>
       </c>
       <c r="L4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="9"/>
-      <c r="N4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="7" t="n">
+      <c r="O4" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="6" t="n">
+      <c r="P4" s="9"/>
+      <c r="Q4" s="7" t="n">
         <v>43467</v>
       </c>
       <c r="R4" s="5"/>
       <c r="S4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
@@ -783,12 +789,12 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
-      <c r="AB4" s="6" t="n">
+      <c r="AB4" s="7" t="n">
         <v>43467</v>
       </c>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AE4" s="5"/>
       <c r="AF4" s="5" t="n">
@@ -797,25 +803,28 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="R5" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="R5" s="0" t="s">
+      <c r="AA5" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="AA5" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>70</v>
-      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AF1"/>

</xml_diff>